<commit_message>
Set hardcoded instead of dynamic (today) date for parameter
This is needed because otherwise the report looks different each day
and thus cannot be used for tests where the report result is compared.
</commit_message>
<xml_diff>
--- a/tests/data/guides/08_expressions/report.xlsx
+++ b/tests/data/guides/08_expressions/report.xlsx
@@ -40,7 +40,7 @@
     <t>Apple (available)</t>
   </si>
   <si>
-    <t>14/May/2023</t>
+    <t>11/May/2023</t>
   </si>
   <si>
     <t>0.49</t>
@@ -64,7 +64,7 @@
     <t>Onions</t>
   </si>
   <si>
-    <t>25/May/2023</t>
+    <t>22/May/2023</t>
   </si>
   <si>
     <t>0.12</t>

</xml_diff>